<commit_message>
Addapted for 2.4 .exe build.
</commit_message>
<xml_diff>
--- a/Templates/TC_template.xlsx
+++ b/Templates/TC_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andmra2\Desktop\Desktop\AnalizaFmeritev\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andmra2\Desktop\Desktop\Python\AFM\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Poročilo" sheetId="1" r:id="rId1"/>
@@ -1454,13 +1454,106 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1469,13 +1562,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1527,24 +1623,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1559,16 +1637,16 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1580,89 +1658,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2093,7 +2093,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="340865120"/>
@@ -2185,7 +2185,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="340864728"/>
@@ -2288,7 +2288,7 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="264017432"/>
@@ -2344,7 +2344,7 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="sl-SI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2705,6 +2705,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
@@ -2743,6 +2744,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
@@ -2759,6 +2761,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2794,6 +2797,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2825,7 +2829,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sl-SI"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2968,7 +2972,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="183457616"/>
@@ -3028,7 +3032,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sl-SI"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="183457288"/>
@@ -3080,7 +3084,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="sl-SI"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4157,7 +4161,7 @@
   </sheetPr>
   <dimension ref="A1:U96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="P93" sqref="P93"/>
     </sheetView>
   </sheetViews>
@@ -4177,54 +4181,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="169"/>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
-      <c r="G1" s="169"/>
-      <c r="H1" s="169"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="171"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="121"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="179"/>
-      <c r="B2" s="180"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="180"/>
-      <c r="F2" s="181"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="144"/>
+      <c r="A2" s="129"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="139"/>
+      <c r="K2" s="139"/>
+      <c r="L2" s="139"/>
+      <c r="M2" s="139"/>
+      <c r="N2" s="140"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="182"/>
-      <c r="B3" s="183"/>
-      <c r="C3" s="183"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="183"/>
-      <c r="F3" s="184"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="146"/>
-      <c r="I3" s="146"/>
-      <c r="J3" s="146"/>
-      <c r="K3" s="146"/>
-      <c r="L3" s="146"/>
-      <c r="M3" s="146"/>
-      <c r="N3" s="147"/>
+      <c r="A3" s="132"/>
+      <c r="B3" s="133"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="142"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="143"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -4269,12 +4273,12 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="175" t="s">
+      <c r="I6" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="175"/>
-      <c r="K6" s="175"/>
-      <c r="L6" s="175"/>
+      <c r="J6" s="125"/>
+      <c r="K6" s="125"/>
+      <c r="L6" s="125"/>
       <c r="M6" s="10"/>
       <c r="N6" s="6"/>
     </row>
@@ -4282,17 +4286,17 @@
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="177" t="s">
+      <c r="D7" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="177"/>
-      <c r="F7" s="178"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="128"/>
       <c r="G7" s="111"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="176"/>
-      <c r="J7" s="177"/>
-      <c r="K7" s="177"/>
-      <c r="L7" s="178"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="127"/>
+      <c r="K7" s="127"/>
+      <c r="L7" s="128"/>
       <c r="M7" s="111"/>
       <c r="N7" s="6"/>
     </row>
@@ -4300,19 +4304,19 @@
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="161" t="s">
+      <c r="D8" s="135" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="161"/>
-      <c r="F8" s="161"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="135"/>
       <c r="G8" s="10"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="161" t="s">
+      <c r="I8" s="135" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="161"/>
-      <c r="K8" s="161"/>
-      <c r="L8" s="161"/>
+      <c r="J8" s="135"/>
+      <c r="K8" s="135"/>
+      <c r="L8" s="135"/>
       <c r="M8" s="10"/>
       <c r="N8" s="6"/>
     </row>
@@ -4320,15 +4324,15 @@
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="162"/>
-      <c r="E9" s="162"/>
-      <c r="F9" s="163"/>
+      <c r="D9" s="148"/>
+      <c r="E9" s="148"/>
+      <c r="F9" s="149"/>
       <c r="G9" s="117"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="187"/>
-      <c r="J9" s="164"/>
-      <c r="K9" s="164"/>
-      <c r="L9" s="165"/>
+      <c r="I9" s="144"/>
+      <c r="J9" s="145"/>
+      <c r="K9" s="145"/>
+      <c r="L9" s="146"/>
       <c r="M9" s="112"/>
       <c r="N9" s="6"/>
     </row>
@@ -4336,11 +4340,11 @@
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="161" t="s">
+      <c r="D10" s="135" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="161"/>
-      <c r="F10" s="161"/>
+      <c r="E10" s="135"/>
+      <c r="F10" s="135"/>
       <c r="G10" s="10"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -4354,9 +4358,9 @@
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="164"/>
-      <c r="E11" s="164"/>
-      <c r="F11" s="165"/>
+      <c r="D11" s="145"/>
+      <c r="E11" s="145"/>
+      <c r="F11" s="146"/>
       <c r="G11" s="112"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -4417,20 +4421,20 @@
       <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="120" t="s">
+      <c r="A15" s="150" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="153"/>
-      <c r="C15" s="153"/>
-      <c r="D15" s="121"/>
-      <c r="E15" s="166" t="s">
+      <c r="B15" s="151"/>
+      <c r="C15" s="151"/>
+      <c r="D15" s="152"/>
+      <c r="E15" s="156" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="166" t="s">
+      <c r="F15" s="156" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="120"/>
-      <c r="H15" s="121"/>
+      <c r="G15" s="150"/>
+      <c r="H15" s="152"/>
       <c r="I15" s="94">
         <v>1</v>
       </c>
@@ -4447,48 +4451,48 @@
       <c r="N15" s="6"/>
     </row>
     <row r="16" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="122"/>
-      <c r="B16" s="155"/>
-      <c r="C16" s="155"/>
-      <c r="D16" s="123"/>
-      <c r="E16" s="167"/>
-      <c r="F16" s="167"/>
-      <c r="G16" s="122"/>
-      <c r="H16" s="123"/>
-      <c r="I16" s="185" t="s">
+      <c r="A16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="157"/>
+      <c r="F16" s="157"/>
+      <c r="G16" s="153"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="136" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="185" t="s">
+      <c r="J16" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="185" t="s">
+      <c r="K16" s="136" t="s">
         <v>69</v>
       </c>
-      <c r="L16" s="185" t="s">
+      <c r="L16" s="136" t="s">
         <v>70</v>
       </c>
       <c r="M16" s="114"/>
       <c r="N16" s="6"/>
     </row>
     <row r="17" spans="1:21" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="172" t="s">
+      <c r="A17" s="122" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="173"/>
-      <c r="C17" s="173"/>
-      <c r="D17" s="174"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="124"/>
       <c r="E17" s="96" t="s">
         <v>71</v>
       </c>
       <c r="F17" s="96" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="124"/>
-      <c r="H17" s="125"/>
-      <c r="I17" s="186"/>
-      <c r="J17" s="186"/>
-      <c r="K17" s="186"/>
-      <c r="L17" s="186"/>
+      <c r="G17" s="180"/>
+      <c r="H17" s="182"/>
+      <c r="I17" s="137"/>
+      <c r="J17" s="137"/>
+      <c r="K17" s="137"/>
+      <c r="L17" s="137"/>
       <c r="M17" s="114"/>
       <c r="N17" s="6"/>
       <c r="Q17"/>
@@ -4508,10 +4512,10 @@
       <c r="F18" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="118" t="s">
+      <c r="G18" s="186" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="119"/>
+      <c r="H18" s="187"/>
       <c r="I18" s="93">
         <f ca="1">'Meritve 800-1100'!V12</f>
         <v>0</v>
@@ -4537,12 +4541,12 @@
       <c r="U18"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="129" t="s">
+      <c r="A19" s="161" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="130"/>
-      <c r="C19" s="130"/>
-      <c r="D19" s="131"/>
+      <c r="B19" s="162"/>
+      <c r="C19" s="162"/>
+      <c r="D19" s="163"/>
       <c r="E19" s="98">
         <f>'Meritev 11V-2s 5V-58s'!AB8</f>
         <v>0</v>
@@ -4551,10 +4555,10 @@
         <f>'Meritev 11V-2s 5V-58s'!AB9</f>
         <v>0</v>
       </c>
-      <c r="G19" s="118" t="s">
+      <c r="G19" s="186" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="119"/>
+      <c r="H19" s="187"/>
       <c r="I19" s="64">
         <f ca="1">'Meritve 800-1100'!V13</f>
         <v>0</v>
@@ -4590,10 +4594,10 @@
       <c r="F20" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="118" t="s">
+      <c r="G20" s="186" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="119"/>
+      <c r="H20" s="187"/>
       <c r="I20" s="65">
         <f ca="1">'Meritve 800-1100'!V14</f>
         <v>0</v>
@@ -4619,12 +4623,12 @@
       <c r="U20"/>
     </row>
     <row r="21" spans="1:21" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="129" t="s">
+      <c r="A21" s="161" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="130"/>
-      <c r="C21" s="130"/>
-      <c r="D21" s="131"/>
+      <c r="B21" s="162"/>
+      <c r="C21" s="162"/>
+      <c r="D21" s="163"/>
       <c r="E21" s="97">
         <f ca="1">'Meritev 11V-2s 5V-58s'!AB3</f>
         <v>0</v>
@@ -4633,10 +4637,10 @@
         <f ca="1">'Meritev 11V-2s 5V-58s'!AB5</f>
         <v>0</v>
       </c>
-      <c r="G21" s="118" t="s">
+      <c r="G21" s="186" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="119"/>
+      <c r="H21" s="187"/>
       <c r="I21" s="65">
         <f ca="1">'Meritve 800-1100'!V15</f>
         <v>0</v>
@@ -4666,20 +4670,20 @@
       <c r="B22" s="110"/>
       <c r="C22" s="95"/>
       <c r="D22" s="25"/>
-      <c r="E22" s="160" t="s">
+      <c r="E22" s="147" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="160"/>
-      <c r="G22" s="157" t="s">
+      <c r="F22" s="147"/>
+      <c r="G22" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="135"/>
-      <c r="I22" s="135"/>
-      <c r="J22" s="135"/>
-      <c r="K22" s="135" t="s">
+      <c r="H22" s="167"/>
+      <c r="I22" s="167"/>
+      <c r="J22" s="167"/>
+      <c r="K22" s="167" t="s">
         <v>30</v>
       </c>
-      <c r="L22" s="135"/>
+      <c r="L22" s="167"/>
       <c r="M22" s="102"/>
       <c r="N22" s="6"/>
       <c r="Q22"/>
@@ -4695,12 +4699,12 @@
       <c r="D23" s="27"/>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
-      <c r="G23" s="158"/>
-      <c r="H23" s="159"/>
-      <c r="I23" s="159"/>
-      <c r="J23" s="159"/>
-      <c r="K23" s="130"/>
-      <c r="L23" s="130"/>
+      <c r="G23" s="184"/>
+      <c r="H23" s="185"/>
+      <c r="I23" s="185"/>
+      <c r="J23" s="185"/>
+      <c r="K23" s="162"/>
+      <c r="L23" s="162"/>
       <c r="M23" s="102"/>
       <c r="N23" s="6"/>
       <c r="R23"/>
@@ -5043,21 +5047,21 @@
       <c r="N42" s="6"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="148" t="s">
+      <c r="A43" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="149"/>
-      <c r="C43" s="149"/>
-      <c r="D43" s="149"/>
-      <c r="E43" s="150"/>
+      <c r="B43" s="175"/>
+      <c r="C43" s="175"/>
+      <c r="D43" s="175"/>
+      <c r="E43" s="176"/>
       <c r="F43" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G43" s="148" t="s">
+      <c r="G43" s="174" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="149"/>
-      <c r="I43" s="150"/>
+      <c r="H43" s="175"/>
+      <c r="I43" s="176"/>
       <c r="J43" s="22" t="s">
         <v>33</v>
       </c>
@@ -5085,38 +5089,38 @@
       <c r="N44" s="15"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="142" t="s">
+      <c r="A45" s="138" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="143"/>
-      <c r="C45" s="143"/>
-      <c r="D45" s="143"/>
-      <c r="E45" s="143"/>
-      <c r="F45" s="144"/>
-      <c r="G45" s="142"/>
-      <c r="H45" s="143"/>
-      <c r="I45" s="143"/>
-      <c r="J45" s="143"/>
-      <c r="K45" s="143"/>
-      <c r="L45" s="143"/>
-      <c r="M45" s="143"/>
-      <c r="N45" s="144"/>
+      <c r="B45" s="139"/>
+      <c r="C45" s="139"/>
+      <c r="D45" s="139"/>
+      <c r="E45" s="139"/>
+      <c r="F45" s="140"/>
+      <c r="G45" s="138"/>
+      <c r="H45" s="139"/>
+      <c r="I45" s="139"/>
+      <c r="J45" s="139"/>
+      <c r="K45" s="139"/>
+      <c r="L45" s="139"/>
+      <c r="M45" s="139"/>
+      <c r="N45" s="140"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="145"/>
-      <c r="B46" s="146"/>
-      <c r="C46" s="146"/>
-      <c r="D46" s="146"/>
-      <c r="E46" s="146"/>
-      <c r="F46" s="147"/>
-      <c r="G46" s="145"/>
-      <c r="H46" s="146"/>
-      <c r="I46" s="146"/>
-      <c r="J46" s="146"/>
-      <c r="K46" s="146"/>
-      <c r="L46" s="146"/>
-      <c r="M46" s="146"/>
-      <c r="N46" s="147"/>
+      <c r="A46" s="141"/>
+      <c r="B46" s="142"/>
+      <c r="C46" s="142"/>
+      <c r="D46" s="142"/>
+      <c r="E46" s="142"/>
+      <c r="F46" s="143"/>
+      <c r="G46" s="141"/>
+      <c r="H46" s="142"/>
+      <c r="I46" s="142"/>
+      <c r="J46" s="142"/>
+      <c r="K46" s="142"/>
+      <c r="L46" s="142"/>
+      <c r="M46" s="142"/>
+      <c r="N46" s="143"/>
     </row>
     <row r="47" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="85" t="s">
@@ -5157,15 +5161,15 @@
       <c r="B49" s="35"/>
       <c r="C49" s="36"/>
       <c r="D49" s="109"/>
-      <c r="E49" s="126" t="str">
+      <c r="E49" s="158" t="str">
         <f ca="1">'Meritev 11V-2s 5V-58s'!AA4&amp;"="&amp;'Meritev 11V-2s 5V-58s'!AB4&amp;"°C, at 60s="&amp;'Meritev 11V-2s 5V-58s'!AB5&amp;"°C)"</f>
         <v>Int. temperature (at 2,3s=0°C, at 60s=0°C)</v>
       </c>
-      <c r="F49" s="127"/>
-      <c r="G49" s="127"/>
-      <c r="H49" s="127"/>
-      <c r="I49" s="127"/>
-      <c r="J49" s="128"/>
+      <c r="F49" s="159"/>
+      <c r="G49" s="159"/>
+      <c r="H49" s="159"/>
+      <c r="I49" s="159"/>
+      <c r="J49" s="160"/>
       <c r="K49" s="35"/>
       <c r="L49" s="35"/>
       <c r="M49" s="35"/>
@@ -5278,12 +5282,12 @@
       <c r="C55" s="35"/>
       <c r="D55" s="35"/>
       <c r="E55" s="41"/>
-      <c r="F55" s="151"/>
-      <c r="G55" s="151"/>
-      <c r="H55" s="152"/>
-      <c r="I55" s="152"/>
-      <c r="J55" s="152"/>
-      <c r="K55" s="152"/>
+      <c r="F55" s="177"/>
+      <c r="G55" s="177"/>
+      <c r="H55" s="178"/>
+      <c r="I55" s="178"/>
+      <c r="J55" s="178"/>
+      <c r="K55" s="178"/>
       <c r="L55" s="35"/>
       <c r="M55" s="35"/>
       <c r="N55" s="36"/>
@@ -5733,38 +5737,38 @@
       <c r="N81" s="6"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A82" s="136" t="s">
+      <c r="A82" s="168" t="s">
         <v>12</v>
       </c>
-      <c r="B82" s="137"/>
-      <c r="C82" s="137"/>
-      <c r="D82" s="137"/>
-      <c r="E82" s="137"/>
-      <c r="F82" s="137"/>
-      <c r="G82" s="137"/>
-      <c r="H82" s="137"/>
-      <c r="I82" s="137"/>
-      <c r="J82" s="137"/>
-      <c r="K82" s="137"/>
-      <c r="L82" s="137"/>
-      <c r="M82" s="137"/>
-      <c r="N82" s="138"/>
+      <c r="B82" s="169"/>
+      <c r="C82" s="169"/>
+      <c r="D82" s="169"/>
+      <c r="E82" s="169"/>
+      <c r="F82" s="169"/>
+      <c r="G82" s="169"/>
+      <c r="H82" s="169"/>
+      <c r="I82" s="169"/>
+      <c r="J82" s="169"/>
+      <c r="K82" s="169"/>
+      <c r="L82" s="169"/>
+      <c r="M82" s="169"/>
+      <c r="N82" s="170"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A83" s="139"/>
-      <c r="B83" s="140"/>
-      <c r="C83" s="140"/>
-      <c r="D83" s="140"/>
-      <c r="E83" s="140"/>
-      <c r="F83" s="140"/>
-      <c r="G83" s="140"/>
-      <c r="H83" s="140"/>
-      <c r="I83" s="140"/>
-      <c r="J83" s="140"/>
-      <c r="K83" s="140"/>
-      <c r="L83" s="140"/>
-      <c r="M83" s="140"/>
-      <c r="N83" s="141"/>
+      <c r="A83" s="171"/>
+      <c r="B83" s="172"/>
+      <c r="C83" s="172"/>
+      <c r="D83" s="172"/>
+      <c r="E83" s="172"/>
+      <c r="F83" s="172"/>
+      <c r="G83" s="172"/>
+      <c r="H83" s="172"/>
+      <c r="I83" s="172"/>
+      <c r="J83" s="172"/>
+      <c r="K83" s="172"/>
+      <c r="L83" s="172"/>
+      <c r="M83" s="172"/>
+      <c r="N83" s="173"/>
     </row>
     <row r="84" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
@@ -5904,13 +5908,13 @@
       <c r="G91" s="5"/>
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
-      <c r="J91" s="120" t="s">
+      <c r="J91" s="150" t="s">
         <v>66</v>
       </c>
-      <c r="K91" s="153"/>
-      <c r="L91" s="153"/>
-      <c r="M91" s="153"/>
-      <c r="N91" s="121"/>
+      <c r="K91" s="151"/>
+      <c r="L91" s="151"/>
+      <c r="M91" s="151"/>
+      <c r="N91" s="152"/>
     </row>
     <row r="92" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
@@ -5922,13 +5926,13 @@
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
-      <c r="J92" s="154" t="s">
+      <c r="J92" s="179" t="s">
         <v>80</v>
       </c>
-      <c r="K92" s="155"/>
-      <c r="L92" s="155"/>
-      <c r="M92" s="155"/>
-      <c r="N92" s="123"/>
+      <c r="K92" s="154"/>
+      <c r="L92" s="154"/>
+      <c r="M92" s="154"/>
+      <c r="N92" s="155"/>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
@@ -5940,11 +5944,11 @@
       <c r="G93" s="5"/>
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
-      <c r="J93" s="122"/>
-      <c r="K93" s="155"/>
-      <c r="L93" s="155"/>
-      <c r="M93" s="155"/>
-      <c r="N93" s="123"/>
+      <c r="J93" s="153"/>
+      <c r="K93" s="154"/>
+      <c r="L93" s="154"/>
+      <c r="M93" s="154"/>
+      <c r="N93" s="155"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
@@ -5956,11 +5960,11 @@
       <c r="G94" s="5"/>
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
-      <c r="J94" s="122"/>
-      <c r="K94" s="155"/>
-      <c r="L94" s="155"/>
-      <c r="M94" s="155"/>
-      <c r="N94" s="123"/>
+      <c r="J94" s="153"/>
+      <c r="K94" s="154"/>
+      <c r="L94" s="154"/>
+      <c r="M94" s="154"/>
+      <c r="N94" s="155"/>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
@@ -5972,57 +5976,41 @@
       <c r="G95" s="5"/>
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
-      <c r="J95" s="124"/>
-      <c r="K95" s="156"/>
-      <c r="L95" s="156"/>
-      <c r="M95" s="156"/>
-      <c r="N95" s="125"/>
+      <c r="J95" s="180"/>
+      <c r="K95" s="181"/>
+      <c r="L95" s="181"/>
+      <c r="M95" s="181"/>
+      <c r="N95" s="182"/>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A96" s="132" t="s">
+      <c r="A96" s="164" t="s">
         <v>16</v>
       </c>
-      <c r="B96" s="133"/>
-      <c r="C96" s="133"/>
-      <c r="D96" s="134"/>
-      <c r="E96" s="132" t="s">
+      <c r="B96" s="165"/>
+      <c r="C96" s="165"/>
+      <c r="D96" s="166"/>
+      <c r="E96" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="F96" s="133"/>
-      <c r="G96" s="133"/>
-      <c r="H96" s="133"/>
-      <c r="I96" s="134"/>
-      <c r="J96" s="132" t="s">
+      <c r="F96" s="165"/>
+      <c r="G96" s="165"/>
+      <c r="H96" s="165"/>
+      <c r="I96" s="166"/>
+      <c r="J96" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="K96" s="133"/>
-      <c r="L96" s="133"/>
-      <c r="M96" s="133"/>
-      <c r="N96" s="134"/>
+      <c r="K96" s="165"/>
+      <c r="L96" s="165"/>
+      <c r="M96" s="165"/>
+      <c r="N96" s="166"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="A2:F3"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="G2:N3"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="A15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G15:H17"/>
     <mergeCell ref="E49:J49"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A21:D21"/>
@@ -6039,11 +6027,27 @@
     <mergeCell ref="G22:J23"/>
     <mergeCell ref="G43:I43"/>
     <mergeCell ref="G45:N46"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G15:H17"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="A2:F3"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="G2:N3"/>
+    <mergeCell ref="I9:L9"/>
   </mergeCells>
   <conditionalFormatting sqref="I20">
     <cfRule type="cellIs" dxfId="7" priority="4" operator="notBetween">
@@ -6157,14 +6161,14 @@
       </c>
       <c r="AD3" s="42"/>
       <c r="AE3" s="29"/>
-      <c r="AF3" s="126" t="str">
+      <c r="AF3" s="158" t="str">
         <f ca="1">AA4&amp;"="&amp;AB4&amp;"°C, at 60s="&amp;AB5&amp;"°C)"</f>
         <v>Int. temperature (at 2,3s=0°C, at 60s=0°C)</v>
       </c>
-      <c r="AG3" s="127"/>
-      <c r="AH3" s="127"/>
-      <c r="AI3" s="127"/>
-      <c r="AJ3" s="128"/>
+      <c r="AG3" s="159"/>
+      <c r="AH3" s="159"/>
+      <c r="AI3" s="159"/>
+      <c r="AJ3" s="160"/>
     </row>
     <row r="4" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4"/>
@@ -6182,14 +6186,14 @@
       </c>
       <c r="AD4" s="42"/>
       <c r="AE4" s="29"/>
-      <c r="AF4" s="126" t="str">
+      <c r="AF4" s="158" t="str">
         <f ca="1">AA2&amp;"="&amp;AB2&amp;"°C, at 60s="&amp;AB3&amp;"°C)"</f>
         <v>Surface temperature (at 2,3s=0°C, at 60s=0°C)</v>
       </c>
-      <c r="AG4" s="127"/>
-      <c r="AH4" s="127"/>
-      <c r="AI4" s="127"/>
-      <c r="AJ4" s="128"/>
+      <c r="AG4" s="159"/>
+      <c r="AH4" s="159"/>
+      <c r="AI4" s="159"/>
+      <c r="AJ4" s="160"/>
     </row>
     <row r="5" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5"/>
@@ -6207,14 +6211,14 @@
       </c>
       <c r="AD5" s="42"/>
       <c r="AE5" s="29"/>
-      <c r="AF5" s="126" t="str">
+      <c r="AF5" s="158" t="str">
         <f ca="1">AA6&amp;"="&amp;AB6&amp;"A, current after 60s="&amp;AB7&amp;"A)"</f>
         <v>Current (max current=0A, current after 60s=0A)</v>
       </c>
-      <c r="AG5" s="127"/>
-      <c r="AH5" s="127"/>
-      <c r="AI5" s="127"/>
-      <c r="AJ5" s="128"/>
+      <c r="AG5" s="159"/>
+      <c r="AH5" s="159"/>
+      <c r="AI5" s="159"/>
+      <c r="AJ5" s="160"/>
     </row>
     <row r="6" spans="2:36" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6"/>
@@ -49570,8 +49574,8 @@
   </sheetPr>
   <dimension ref="U1:AA31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E28010"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49625,7 +49629,7 @@
     </row>
     <row r="4" spans="21:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U4" s="75">
-        <f ca="1">INDIRECT("B"&amp;9100+Z3*100)</f>
+        <f ca="1">INDIRECT("B"&amp;14100+Z3*100)</f>
         <v>0</v>
       </c>
       <c r="V4" s="67">
@@ -49639,7 +49643,7 @@
     </row>
     <row r="5" spans="21:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="U5" s="75">
-        <f ca="1">INDIRECT("B"&amp;15200+Z3*100)</f>
+        <f ca="1">INDIRECT("B"&amp;20200+Z3*100)</f>
         <v>0</v>
       </c>
       <c r="V5" s="67">
@@ -49653,7 +49657,7 @@
     </row>
     <row r="6" spans="21:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U6" s="76">
-        <f ca="1">INDIRECT("B"&amp;21300+Z3*100)</f>
+        <f ca="1">INDIRECT("B"&amp;26300+Z3*100)</f>
         <v>0</v>
       </c>
       <c r="V6" s="68">
@@ -49834,6 +49838,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Confidential1 xmlns="82f67884-f2fe-436e-ba3e-f94bce1a90ac">false</Confidential1>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Splošni zapisi" ma:contentTypeID="0x010100F78B00D4F12061488B1E0B05A562A631001B543E2438AD264A879EFE753B7CE596" ma:contentTypeVersion="" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="ee7b47c5fbf7bc47176d407da8b60e16">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="82f67884-f2fe-436e-ba3e-f94bce1a90ac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c835d47d9ed08d550d26c3303fd928d8" ns2:_="">
     <xsd:import namespace="82f67884-f2fe-436e-ba3e-f94bce1a90ac"/>
@@ -49959,37 +49980,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Confidential1 xmlns="82f67884-f2fe-436e-ba3e-f94bce1a90ac">false</Confidential1>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B60684F0-BE92-4FC2-8F38-9CE0938177FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78C4947-E533-419A-963D-FE9C69FB2FCE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="82f67884-f2fe-436e-ba3e-f94bce1a90ac"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -50011,9 +50005,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78C4947-E533-419A-963D-FE9C69FB2FCE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B60684F0-BE92-4FC2-8F38-9CE0938177FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="82f67884-f2fe-436e-ba3e-f94bce1a90ac"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>